<commit_message>
bigger databse + better output formaat
</commit_message>
<xml_diff>
--- a/похожие тексты.xlsx
+++ b/похожие тексты.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,15 +436,20 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>names</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>text</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>tokens</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>int strvis(undefined2 *param_1,char *param_2,uint param_3)
 {
@@ -468,7 +473,7 @@
 }</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>void alerts_ring_bell(undefined4 param_1,undefined4 param_2,undefined4 param_3,undefined4 param_4,
                      undefined4 param_5,undefined4 param_6,undefined4 param_7,undefined4 param_8,
@@ -499,7 +504,7 @@
 }</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>sum</t>
         </is>
@@ -510,6 +515,11 @@
         <v>0</v>
       </c>
       <c r="B2" t="inlineStr">
+        <is>
+          <t>strvisx</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
         <is>
           <t>int
 strvisx(char *dst, const char *src, size_t len, int flag)
@@ -527,18 +537,18 @@
 }</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>['int', 'strvisx', 'char', 'dst', 'const', 'char', 'src', 'size_t', 'len', 'int', 'flag', 'char', 'c', 'char', 'start', 'for', 'start', 'dst', 'len', 'len', 'c', 'src', 'dst', 'vis', 'dst', 'c', 'flag', 'src', 'if', 'len', 'dst', 'vis', 'dst', 'src', 'flag', 'dst', 'return', 'dst', 'start']</t>
         </is>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
         <v>0.19318687915802</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>0.06145553290843964</v>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
         <v>0.2546424120664597</v>
       </c>
     </row>
@@ -547,6 +557,11 @@
         <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
+        <is>
+          <t>strvis_orig</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
         <is>
           <t>int
 strvis(char *dst, const char *src, int flag)
@@ -560,18 +575,18 @@
 }</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>['int', 'strvis', 'char', 'dst', 'const', 'char', 'src', 'int', 'flag', 'char', 'c', 'char', 'start', 'for', 'start', 'dst', 'c', 'src', 'dst', 'vis', 'dst', 'c', 'flag', 'src', 'dst', 'return', 'dst', 'start']</t>
         </is>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
         <v>0.2620097994804382</v>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>0.07766927778720856</v>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
         <v>0.3396790772676468</v>
       </c>
     </row>
@@ -580,6 +595,11 @@
         <v>4</v>
       </c>
       <c r="B4" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
         <is>
           <t>void
 alerts_ring_bell(struct session *s)
@@ -592,18 +612,18 @@
 }</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>['void', 'alerts_ring_bell', 'struct', 'session', 's', 'struct', 'client', 'c', 'TAILQ_FOREACH', 'c', 'clients', 'entry', 'if', 'c', 'session', 's', 'c', 'flags', 'CLIENT_CONTROL', 'tty_putcode', 'c', 'tty', 'TTYC_BEL']</t>
         </is>
       </c>
-      <c r="D4" t="n">
+      <c r="E4" t="n">
         <v>0.007051536813378334</v>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
         <v>0.4579939544200897</v>
       </c>
-      <c r="F4" t="n">
+      <c r="G4" t="n">
         <v>0.4650454912334681</v>
       </c>
     </row>

</xml_diff>